<commit_message>
add password storage, raised fail threshold
</commit_message>
<xml_diff>
--- a/geography/basins_searchterms_tracking.xlsx
+++ b/geography/basins_searchterms_tracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shared Waters Lab\geography\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shared Waters Lab\geography\geography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6F8BB-82C8-4DC2-9DB8-83F7FBBE83B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BCC466-A63B-4A5E-A786-2345F86EBF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3180,10 +3180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3489,11 +3495,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M277" sqref="M277"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="4" max="4" width="87.07421875" style="3" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
@@ -3502,7 +3511,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -3528,14 +3537,14 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3545,7 +3554,7 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
@@ -3565,7 +3574,7 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
@@ -3582,14 +3591,14 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3599,7 +3608,7 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F6" t="s">
@@ -3609,7 +3618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3619,14 +3628,14 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3636,7 +3645,7 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
@@ -3656,7 +3665,7 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H9" t="s">
@@ -3673,7 +3682,7 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H10" t="s">
@@ -3690,7 +3699,7 @@
       <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
@@ -3700,7 +3709,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3710,7 +3719,7 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
       <c r="H12" t="s">
@@ -3727,14 +3736,14 @@
       <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="H13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="204" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3744,7 +3753,7 @@
       <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F14" t="s">
@@ -3764,7 +3773,7 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H15" t="s">
@@ -3781,7 +3790,7 @@
       <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>61</v>
       </c>
       <c r="H16" t="s">
@@ -3798,14 +3807,14 @@
       <c r="C17" t="s">
         <v>63</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3815,7 +3824,7 @@
       <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F18" t="s">
@@ -3825,7 +3834,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3835,7 +3844,7 @@
       <c r="C19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F19" t="s">
@@ -3845,7 +3854,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3855,7 +3864,7 @@
       <c r="C20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F20" t="s">
@@ -3865,7 +3874,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3875,7 +3884,7 @@
       <c r="C21" t="s">
         <v>76</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H21" t="s">
@@ -3892,7 +3901,7 @@
       <c r="C22" t="s">
         <v>80</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H22" t="s">
@@ -3909,14 +3918,14 @@
       <c r="C23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3926,7 +3935,7 @@
       <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F24" t="s">
@@ -3946,7 +3955,7 @@
       <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F25" t="s">
@@ -3966,14 +3975,14 @@
       <c r="C26" t="s">
         <v>94</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3983,7 +3992,7 @@
       <c r="C27" t="s">
         <v>97</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F27" t="s">
@@ -4003,14 +4012,14 @@
       <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>101</v>
       </c>
       <c r="H28" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4020,7 +4029,7 @@
       <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F29" t="s">
@@ -4040,14 +4049,14 @@
       <c r="C30" t="s">
         <v>108</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>108</v>
       </c>
       <c r="H30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4057,7 +4066,7 @@
       <c r="C31" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>111</v>
       </c>
       <c r="F31" t="s">
@@ -4077,7 +4086,7 @@
       <c r="C32" t="s">
         <v>114</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>114</v>
       </c>
       <c r="F32" t="s">
@@ -4097,14 +4106,14 @@
       <c r="C33" t="s">
         <v>116</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>116</v>
       </c>
       <c r="H33" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4114,7 +4123,7 @@
       <c r="C34" t="s">
         <v>119</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>120</v>
       </c>
       <c r="F34" t="s">
@@ -4134,7 +4143,7 @@
       <c r="C35" t="s">
         <v>123</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
         <v>123</v>
       </c>
       <c r="H35" t="s">
@@ -4151,7 +4160,7 @@
       <c r="C36" t="s">
         <v>125</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H36" t="s">
@@ -4168,7 +4177,7 @@
       <c r="C37" t="s">
         <v>129</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F37" t="s">
@@ -4178,7 +4187,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4188,7 +4197,7 @@
       <c r="C38" t="s">
         <v>133</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="3" t="s">
         <v>134</v>
       </c>
       <c r="F38" t="s">
@@ -4208,7 +4217,7 @@
       <c r="C39" t="s">
         <v>137</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>138</v>
       </c>
       <c r="F39" t="s">
@@ -4218,7 +4227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4228,7 +4237,7 @@
       <c r="C40" t="s">
         <v>140</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="3" t="s">
         <v>141</v>
       </c>
       <c r="F40" t="s">
@@ -4238,7 +4247,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4248,7 +4257,7 @@
       <c r="C41" t="s">
         <v>144</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
       <c r="F41" t="s">
@@ -4268,7 +4277,7 @@
       <c r="C42" t="s">
         <v>148</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>149</v>
       </c>
       <c r="F42" t="s">
@@ -4278,7 +4287,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="291.45" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4288,7 +4297,7 @@
       <c r="C43" t="s">
         <v>152</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="3" t="s">
         <v>153</v>
       </c>
       <c r="H43" t="s">
@@ -4305,14 +4314,14 @@
       <c r="C44" t="s">
         <v>156</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="3" t="s">
         <v>156</v>
       </c>
       <c r="H44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4322,14 +4331,14 @@
       <c r="C45" t="s">
         <v>158</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="3" t="s">
         <v>159</v>
       </c>
       <c r="H45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4339,7 +4348,7 @@
       <c r="C46" t="s">
         <v>161</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="3" t="s">
         <v>162</v>
       </c>
       <c r="F46" t="s">
@@ -4349,7 +4358,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4359,7 +4368,7 @@
       <c r="C47" t="s">
         <v>165</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="3" t="s">
         <v>166</v>
       </c>
       <c r="F47" t="s">
@@ -4379,14 +4388,14 @@
       <c r="C48" t="s">
         <v>169</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="3" t="s">
         <v>169</v>
       </c>
       <c r="H48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4396,7 +4405,7 @@
       <c r="C49" t="s">
         <v>171</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="3" t="s">
         <v>172</v>
       </c>
       <c r="F49" t="s">
@@ -4406,7 +4415,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4416,7 +4425,7 @@
       <c r="C50" t="s">
         <v>175</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="3" t="s">
         <v>176</v>
       </c>
       <c r="F50" t="s">
@@ -4436,7 +4445,7 @@
       <c r="C51" t="s">
         <v>178</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="3" t="s">
         <v>179</v>
       </c>
       <c r="F51" t="s">
@@ -4456,14 +4465,14 @@
       <c r="C52" t="s">
         <v>181</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="3" t="s">
         <v>182</v>
       </c>
       <c r="H52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4473,7 +4482,7 @@
       <c r="C53" t="s">
         <v>184</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="3" t="s">
         <v>185</v>
       </c>
       <c r="F53" t="s">
@@ -4483,7 +4492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4493,7 +4502,7 @@
       <c r="C54" t="s">
         <v>187</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="3" t="s">
         <v>188</v>
       </c>
       <c r="F54" t="s">
@@ -4513,7 +4522,7 @@
       <c r="C55" t="s">
         <v>191</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="3" t="s">
         <v>191</v>
       </c>
       <c r="H55" t="s">
@@ -4530,7 +4539,7 @@
       <c r="C56" t="s">
         <v>194</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="3" t="s">
         <v>194</v>
       </c>
       <c r="H56" t="s">
@@ -4547,7 +4556,7 @@
       <c r="C57" t="s">
         <v>196</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="3" t="s">
         <v>197</v>
       </c>
       <c r="F57" t="s">
@@ -4567,7 +4576,7 @@
       <c r="C58" t="s">
         <v>200</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="3" t="s">
         <v>201</v>
       </c>
       <c r="F58" t="s">
@@ -4587,14 +4596,14 @@
       <c r="C59" t="s">
         <v>203</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="3" t="s">
         <v>203</v>
       </c>
       <c r="H59" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4604,7 +4613,7 @@
       <c r="C60" t="s">
         <v>206</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="3" t="s">
         <v>207</v>
       </c>
       <c r="F60" t="s">
@@ -4624,7 +4633,7 @@
       <c r="C61" t="s">
         <v>210</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="3" t="s">
         <v>210</v>
       </c>
       <c r="F61" t="s">
@@ -4634,7 +4643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4644,7 +4653,7 @@
       <c r="C62" t="s">
         <v>212</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F62" t="s">
@@ -4654,7 +4663,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4664,14 +4673,14 @@
       <c r="C63" t="s">
         <v>216</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="3" t="s">
         <v>217</v>
       </c>
       <c r="H63" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4681,7 +4690,7 @@
       <c r="C64" t="s">
         <v>220</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="3" t="s">
         <v>221</v>
       </c>
       <c r="F64" t="s">
@@ -4701,14 +4710,14 @@
       <c r="C65" t="s">
         <v>224</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="3" t="s">
         <v>224</v>
       </c>
       <c r="H65" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4718,7 +4727,7 @@
       <c r="C66" t="s">
         <v>227</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="3" t="s">
         <v>228</v>
       </c>
       <c r="H66" t="s">
@@ -4735,14 +4744,14 @@
       <c r="C67" t="s">
         <v>231</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="3" t="s">
         <v>232</v>
       </c>
       <c r="H67" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4752,7 +4761,7 @@
       <c r="C68" t="s">
         <v>235</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="3" t="s">
         <v>236</v>
       </c>
       <c r="H68" t="s">
@@ -4769,14 +4778,14 @@
       <c r="C69" t="s">
         <v>239</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="3" t="s">
         <v>239</v>
       </c>
       <c r="H69" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4786,7 +4795,7 @@
       <c r="C70" t="s">
         <v>242</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="3" t="s">
         <v>243</v>
       </c>
       <c r="F70" t="s">
@@ -4796,7 +4805,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4806,7 +4815,7 @@
       <c r="C71" t="s">
         <v>245</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="3" t="s">
         <v>246</v>
       </c>
       <c r="H71" t="s">
@@ -4823,14 +4832,14 @@
       <c r="C72" t="s">
         <v>249</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="3" t="s">
         <v>249</v>
       </c>
       <c r="H72" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4840,14 +4849,14 @@
       <c r="C73" t="s">
         <v>251</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="3" t="s">
         <v>252</v>
       </c>
       <c r="H73" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4857,14 +4866,14 @@
       <c r="C74" t="s">
         <v>255</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H74" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4874,14 +4883,14 @@
       <c r="C75" t="s">
         <v>259</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="3" t="s">
         <v>260</v>
       </c>
       <c r="H75" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4891,7 +4900,7 @@
       <c r="C76" t="s">
         <v>263</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="3" t="s">
         <v>264</v>
       </c>
       <c r="H76" t="s">
@@ -4908,7 +4917,7 @@
       <c r="C77" t="s">
         <v>267</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H77" t="s">
@@ -4925,14 +4934,14 @@
       <c r="C78" t="s">
         <v>269</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="3" t="s">
         <v>270</v>
       </c>
       <c r="H78" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4942,7 +4951,7 @@
       <c r="C79" t="s">
         <v>272</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="3" t="s">
         <v>273</v>
       </c>
       <c r="F79" t="s">
@@ -4952,7 +4961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4962,7 +4971,7 @@
       <c r="C80" t="s">
         <v>275</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="3" t="s">
         <v>276</v>
       </c>
       <c r="F80" t="s">
@@ -4982,7 +4991,7 @@
       <c r="C81" t="s">
         <v>279</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="3" t="s">
         <v>279</v>
       </c>
       <c r="H81" t="s">
@@ -4999,7 +5008,7 @@
       <c r="C82" t="s">
         <v>281</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="3" t="s">
         <v>282</v>
       </c>
       <c r="H82" t="s">
@@ -5016,7 +5025,7 @@
       <c r="C83" t="s">
         <v>284</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="3" t="s">
         <v>285</v>
       </c>
       <c r="H83" t="s">
@@ -5033,7 +5042,7 @@
       <c r="C84" t="s">
         <v>287</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="3" t="s">
         <v>287</v>
       </c>
       <c r="H84" t="s">
@@ -5050,14 +5059,14 @@
       <c r="C85" t="s">
         <v>290</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="3" t="s">
         <v>290</v>
       </c>
       <c r="H85" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5067,7 +5076,7 @@
       <c r="C86" t="s">
         <v>292</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="3" t="s">
         <v>293</v>
       </c>
       <c r="H86" t="s">
@@ -5084,14 +5093,14 @@
       <c r="C87" t="s">
         <v>295</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="3" t="s">
         <v>296</v>
       </c>
       <c r="H87" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5101,7 +5110,7 @@
       <c r="C88" t="s">
         <v>298</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F88" t="s">
@@ -5111,7 +5120,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" ht="276.89999999999998" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5121,7 +5130,7 @@
       <c r="C89" t="s">
         <v>301</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="3" t="s">
         <v>302</v>
       </c>
       <c r="F89" t="s">
@@ -5131,7 +5140,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" ht="276.89999999999998" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5141,7 +5150,7 @@
       <c r="C90" t="s">
         <v>305</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="3" t="s">
         <v>306</v>
       </c>
       <c r="H90" t="s">
@@ -5158,7 +5167,7 @@
       <c r="C91" t="s">
         <v>309</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="3" t="s">
         <v>310</v>
       </c>
       <c r="F91" t="s">
@@ -5168,7 +5177,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5178,7 +5187,7 @@
       <c r="C92" t="s">
         <v>313</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="3" t="s">
         <v>314</v>
       </c>
       <c r="F92" t="s">
@@ -5188,7 +5197,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:8" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5198,7 +5207,7 @@
       <c r="C93" t="s">
         <v>317</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="3" t="s">
         <v>318</v>
       </c>
       <c r="F93" t="s">
@@ -5218,14 +5227,14 @@
       <c r="C94" t="s">
         <v>321</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="3" t="s">
         <v>321</v>
       </c>
       <c r="H94" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5235,7 +5244,7 @@
       <c r="C95" t="s">
         <v>323</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="3" t="s">
         <v>324</v>
       </c>
       <c r="F95" t="s">
@@ -5255,14 +5264,14 @@
       <c r="C96" t="s">
         <v>327</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="3" t="s">
         <v>327</v>
       </c>
       <c r="H96" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5272,7 +5281,7 @@
       <c r="C97" t="s">
         <v>330</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="3" t="s">
         <v>331</v>
       </c>
       <c r="F97" t="s">
@@ -5282,7 +5291,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5292,7 +5301,7 @@
       <c r="C98" t="s">
         <v>334</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="3" t="s">
         <v>335</v>
       </c>
       <c r="H98" t="s">
@@ -5309,14 +5318,14 @@
       <c r="C99" t="s">
         <v>337</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="3" t="s">
         <v>337</v>
       </c>
       <c r="H99" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5326,7 +5335,7 @@
       <c r="C100" t="s">
         <v>339</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="3" t="s">
         <v>340</v>
       </c>
       <c r="F100" t="s">
@@ -5346,14 +5355,14 @@
       <c r="C101" t="s">
         <v>343</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="3" t="s">
         <v>343</v>
       </c>
       <c r="H101" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -5363,7 +5372,7 @@
       <c r="C102" t="s">
         <v>345</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="3" t="s">
         <v>346</v>
       </c>
       <c r="F102" t="s">
@@ -5383,14 +5392,14 @@
       <c r="C103" t="s">
         <v>348</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="3" t="s">
         <v>348</v>
       </c>
       <c r="H103" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -5400,7 +5409,7 @@
       <c r="C104" t="s">
         <v>351</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="3" t="s">
         <v>352</v>
       </c>
       <c r="H104" t="s">
@@ -5417,7 +5426,7 @@
       <c r="C105" t="s">
         <v>355</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="3" t="s">
         <v>356</v>
       </c>
       <c r="H105" t="s">
@@ -5434,14 +5443,14 @@
       <c r="C106" t="s">
         <v>358</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="3" t="s">
         <v>359</v>
       </c>
       <c r="H106" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -5451,14 +5460,14 @@
       <c r="C107" t="s">
         <v>361</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="3" t="s">
         <v>362</v>
       </c>
       <c r="H107" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -5468,7 +5477,7 @@
       <c r="C108" t="s">
         <v>364</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="3" t="s">
         <v>365</v>
       </c>
       <c r="F108" t="s">
@@ -5488,14 +5497,14 @@
       <c r="C109" t="s">
         <v>367</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="3" t="s">
         <v>367</v>
       </c>
       <c r="H109" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -5505,14 +5514,14 @@
       <c r="C110" t="s">
         <v>370</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="3" t="s">
         <v>371</v>
       </c>
       <c r="H110" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5522,7 +5531,7 @@
       <c r="C111" t="s">
         <v>373</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="3" t="s">
         <v>374</v>
       </c>
       <c r="F111" t="s">
@@ -5542,7 +5551,7 @@
       <c r="C112" t="s">
         <v>377</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="3" t="s">
         <v>378</v>
       </c>
       <c r="H112" t="s">
@@ -5559,14 +5568,14 @@
       <c r="C113" t="s">
         <v>381</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="3" t="s">
         <v>381</v>
       </c>
       <c r="H113" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5576,14 +5585,14 @@
       <c r="C114" t="s">
         <v>383</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="3" t="s">
         <v>384</v>
       </c>
       <c r="H114" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5593,7 +5602,7 @@
       <c r="C115" t="s">
         <v>387</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="3" t="s">
         <v>388</v>
       </c>
       <c r="H115" t="s">
@@ -5610,7 +5619,7 @@
       <c r="C116" t="s">
         <v>391</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="3" t="s">
         <v>392</v>
       </c>
       <c r="H116" t="s">
@@ -5627,7 +5636,7 @@
       <c r="C117" t="s">
         <v>395</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="3" t="s">
         <v>395</v>
       </c>
       <c r="H117" t="s">
@@ -5644,14 +5653,14 @@
       <c r="C118" t="s">
         <v>397</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="3" t="s">
         <v>397</v>
       </c>
       <c r="H118" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5661,14 +5670,14 @@
       <c r="C119" t="s">
         <v>400</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="3" t="s">
         <v>401</v>
       </c>
       <c r="H119" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5678,7 +5687,7 @@
       <c r="C120" t="s">
         <v>404</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="3" t="s">
         <v>405</v>
       </c>
       <c r="F120" t="s">
@@ -5688,7 +5697,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5698,7 +5707,7 @@
       <c r="C121" t="s">
         <v>408</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="3" t="s">
         <v>409</v>
       </c>
       <c r="F121" t="s">
@@ -5718,14 +5727,14 @@
       <c r="C122" t="s">
         <v>412</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="3" t="s">
         <v>412</v>
       </c>
       <c r="H122" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5735,7 +5744,7 @@
       <c r="C123" t="s">
         <v>415</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="3" t="s">
         <v>416</v>
       </c>
       <c r="H123" t="s">
@@ -5752,14 +5761,14 @@
       <c r="C124" t="s">
         <v>419</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="3" t="s">
         <v>419</v>
       </c>
       <c r="H124" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5769,7 +5778,7 @@
       <c r="C125" t="s">
         <v>422</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="3" t="s">
         <v>423</v>
       </c>
       <c r="F125" t="s">
@@ -5789,7 +5798,7 @@
       <c r="C126" t="s">
         <v>426</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="3" t="s">
         <v>427</v>
       </c>
       <c r="H126" t="s">
@@ -5806,7 +5815,7 @@
       <c r="C127" t="s">
         <v>429</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="3" t="s">
         <v>429</v>
       </c>
       <c r="H127" t="s">
@@ -5823,7 +5832,7 @@
       <c r="C128" t="s">
         <v>431</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="3" t="s">
         <v>431</v>
       </c>
       <c r="H128" t="s">
@@ -5840,14 +5849,14 @@
       <c r="C129" t="s">
         <v>433</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="3" t="s">
         <v>434</v>
       </c>
       <c r="H129" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5857,7 +5866,7 @@
       <c r="C130" t="s">
         <v>436</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="3" t="s">
         <v>437</v>
       </c>
       <c r="F130" t="s">
@@ -5867,7 +5876,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5877,7 +5886,7 @@
       <c r="C131" t="s">
         <v>439</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="3" t="s">
         <v>440</v>
       </c>
       <c r="H131" t="s">
@@ -5894,7 +5903,7 @@
       <c r="C132" t="s">
         <v>442</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="3" t="s">
         <v>443</v>
       </c>
       <c r="H132" t="s">
@@ -5911,14 +5920,14 @@
       <c r="C133" t="s">
         <v>446</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="3" t="s">
         <v>446</v>
       </c>
       <c r="H133" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5928,7 +5937,7 @@
       <c r="C134" t="s">
         <v>448</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="3" t="s">
         <v>449</v>
       </c>
       <c r="F134" t="s">
@@ -5948,14 +5957,14 @@
       <c r="C135" t="s">
         <v>452</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="3" t="s">
         <v>453</v>
       </c>
       <c r="H135" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5965,7 +5974,7 @@
       <c r="C136" t="s">
         <v>455</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="3" t="s">
         <v>456</v>
       </c>
       <c r="F136" t="s">
@@ -5975,7 +5984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5985,7 +5994,7 @@
       <c r="C137" t="s">
         <v>458</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="3" t="s">
         <v>459</v>
       </c>
       <c r="F137" t="s">
@@ -5995,7 +6004,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -6005,7 +6014,7 @@
       <c r="C138" t="s">
         <v>462</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="3" t="s">
         <v>463</v>
       </c>
       <c r="F138" t="s">
@@ -6015,7 +6024,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -6025,7 +6034,7 @@
       <c r="C139" t="s">
         <v>466</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="3" t="s">
         <v>467</v>
       </c>
       <c r="F139" t="s">
@@ -6045,7 +6054,7 @@
       <c r="C140" t="s">
         <v>470</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="3" t="s">
         <v>471</v>
       </c>
       <c r="F140" t="s">
@@ -6055,7 +6064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -6065,7 +6074,7 @@
       <c r="C141" t="s">
         <v>473</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="3" t="s">
         <v>474</v>
       </c>
       <c r="F141" t="s">
@@ -6075,7 +6084,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -6085,7 +6094,7 @@
       <c r="C142" t="s">
         <v>476</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="3" t="s">
         <v>477</v>
       </c>
       <c r="F142" t="s">
@@ -6095,7 +6104,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -6105,7 +6114,7 @@
       <c r="C143" t="s">
         <v>479</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="3" t="s">
         <v>480</v>
       </c>
       <c r="F143" t="s">
@@ -6115,7 +6124,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -6125,14 +6134,14 @@
       <c r="C144" t="s">
         <v>482</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="3" t="s">
         <v>483</v>
       </c>
       <c r="H144" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -6142,7 +6151,7 @@
       <c r="C145" t="s">
         <v>486</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="3" t="s">
         <v>487</v>
       </c>
       <c r="F145" t="s">
@@ -6162,14 +6171,14 @@
       <c r="C146" t="s">
         <v>490</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="3" t="s">
         <v>490</v>
       </c>
       <c r="H146" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -6179,7 +6188,7 @@
       <c r="C147" t="s">
         <v>493</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="3" t="s">
         <v>494</v>
       </c>
       <c r="F147" t="s">
@@ -6189,7 +6198,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:8" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -6199,7 +6208,7 @@
       <c r="C148" t="s">
         <v>497</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="3" t="s">
         <v>498</v>
       </c>
       <c r="F148" t="s">
@@ -6219,14 +6228,14 @@
       <c r="C149" t="s">
         <v>500</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="3" t="s">
         <v>501</v>
       </c>
       <c r="H149" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -6236,7 +6245,7 @@
       <c r="C150" t="s">
         <v>503</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="3" t="s">
         <v>504</v>
       </c>
       <c r="H150" t="s">
@@ -6253,14 +6262,14 @@
       <c r="C151" t="s">
         <v>506</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="3" t="s">
         <v>506</v>
       </c>
       <c r="H151" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -6270,7 +6279,7 @@
       <c r="C152" t="s">
         <v>508</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="3" t="s">
         <v>509</v>
       </c>
       <c r="F152" t="s">
@@ -6280,7 +6289,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -6290,7 +6299,7 @@
       <c r="C153" t="s">
         <v>512</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="3" t="s">
         <v>513</v>
       </c>
       <c r="F153" t="s">
@@ -6300,7 +6309,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -6310,7 +6319,7 @@
       <c r="C154" t="s">
         <v>516</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="3" t="s">
         <v>517</v>
       </c>
       <c r="F154" t="s">
@@ -6330,14 +6339,14 @@
       <c r="C155" t="s">
         <v>519</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="3" t="s">
         <v>519</v>
       </c>
       <c r="H155" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -6347,7 +6356,7 @@
       <c r="C156" t="s">
         <v>522</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="3" t="s">
         <v>523</v>
       </c>
       <c r="F156" t="s">
@@ -6357,7 +6366,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6367,7 +6376,7 @@
       <c r="C157" t="s">
         <v>526</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="3" t="s">
         <v>527</v>
       </c>
       <c r="F157" t="s">
@@ -6377,7 +6386,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6387,7 +6396,7 @@
       <c r="C158" t="s">
         <v>530</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="3" t="s">
         <v>531</v>
       </c>
       <c r="F158" t="s">
@@ -6407,14 +6416,14 @@
       <c r="C159" t="s">
         <v>533</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="3" t="s">
         <v>533</v>
       </c>
       <c r="H159" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6424,7 +6433,7 @@
       <c r="C160" t="s">
         <v>535</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="3" t="s">
         <v>536</v>
       </c>
       <c r="F160" t="s">
@@ -6444,7 +6453,7 @@
       <c r="C161" t="s">
         <v>539</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="3" t="s">
         <v>539</v>
       </c>
       <c r="H161" t="s">
@@ -6461,7 +6470,7 @@
       <c r="C162" t="s">
         <v>541</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="3" t="s">
         <v>542</v>
       </c>
       <c r="F162" t="s">
@@ -6481,14 +6490,14 @@
       <c r="C163" t="s">
         <v>544</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="3" t="s">
         <v>545</v>
       </c>
       <c r="H163" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -6498,7 +6507,7 @@
       <c r="C164" t="s">
         <v>547</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="3" t="s">
         <v>548</v>
       </c>
       <c r="F164" t="s">
@@ -6508,7 +6517,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -6518,7 +6527,7 @@
       <c r="C165" t="s">
         <v>551</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="3" t="s">
         <v>552</v>
       </c>
       <c r="F165" t="s">
@@ -6528,7 +6537,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:8" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -6538,7 +6547,7 @@
       <c r="C166" t="s">
         <v>554</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="3" t="s">
         <v>555</v>
       </c>
       <c r="H166" t="s">
@@ -6555,14 +6564,14 @@
       <c r="C167" t="s">
         <v>558</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="3" t="s">
         <v>559</v>
       </c>
       <c r="H167" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6572,14 +6581,14 @@
       <c r="C168" t="s">
         <v>561</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="3" t="s">
         <v>562</v>
       </c>
       <c r="H168" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:8" ht="320.60000000000002" x14ac:dyDescent="0.4">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6589,7 +6598,7 @@
       <c r="C169" t="s">
         <v>564</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="3" t="s">
         <v>565</v>
       </c>
       <c r="F169" t="s">
@@ -6599,7 +6608,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:8" ht="204" x14ac:dyDescent="0.4">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6609,7 +6618,7 @@
       <c r="C170" t="s">
         <v>568</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="3" t="s">
         <v>569</v>
       </c>
       <c r="H170" t="s">
@@ -6626,14 +6635,14 @@
       <c r="C171" t="s">
         <v>571</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="3" t="s">
         <v>571</v>
       </c>
       <c r="H171" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6643,7 +6652,7 @@
       <c r="C172" t="s">
         <v>573</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="3" t="s">
         <v>574</v>
       </c>
       <c r="F172" t="s">
@@ -6653,7 +6662,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6663,7 +6672,7 @@
       <c r="C173" t="s">
         <v>576</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="3" t="s">
         <v>577</v>
       </c>
       <c r="F173" t="s">
@@ -6673,7 +6682,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6683,7 +6692,7 @@
       <c r="C174" t="s">
         <v>579</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="3" t="s">
         <v>580</v>
       </c>
       <c r="F174" t="s">
@@ -6693,7 +6702,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:8" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6703,7 +6712,7 @@
       <c r="C175" t="s">
         <v>583</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="3" t="s">
         <v>584</v>
       </c>
       <c r="F175" t="s">
@@ -6713,7 +6722,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6723,7 +6732,7 @@
       <c r="C176" t="s">
         <v>587</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="3" t="s">
         <v>588</v>
       </c>
       <c r="F176" t="s">
@@ -6743,14 +6752,14 @@
       <c r="C177" t="s">
         <v>590</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="3" t="s">
         <v>591</v>
       </c>
       <c r="H177" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:8" ht="320.60000000000002" x14ac:dyDescent="0.4">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6760,7 +6769,7 @@
       <c r="C178" t="s">
         <v>594</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="3" t="s">
         <v>595</v>
       </c>
       <c r="F178" t="s">
@@ -6780,14 +6789,14 @@
       <c r="C179" t="s">
         <v>598</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="3" t="s">
         <v>599</v>
       </c>
       <c r="H179" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6797,7 +6806,7 @@
       <c r="C180" t="s">
         <v>602</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="3" t="s">
         <v>603</v>
       </c>
       <c r="F180" t="s">
@@ -6817,7 +6826,7 @@
       <c r="C181" t="s">
         <v>605</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="3" t="s">
         <v>606</v>
       </c>
       <c r="H181" t="s">
@@ -6834,7 +6843,7 @@
       <c r="C182" t="s">
         <v>609</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="3" t="s">
         <v>609</v>
       </c>
       <c r="H182" t="s">
@@ -6851,14 +6860,14 @@
       <c r="C183" t="s">
         <v>612</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="3" t="s">
         <v>612</v>
       </c>
       <c r="H183" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:8" ht="393.45" x14ac:dyDescent="0.4">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6868,7 +6877,7 @@
       <c r="C184" t="s">
         <v>614</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="3" t="s">
         <v>615</v>
       </c>
       <c r="F184" t="s">
@@ -6878,7 +6887,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:8" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6888,14 +6897,14 @@
       <c r="C185" t="s">
         <v>617</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="3" t="s">
         <v>618</v>
       </c>
       <c r="H185" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6905,7 +6914,7 @@
       <c r="C186" t="s">
         <v>620</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="3" t="s">
         <v>621</v>
       </c>
       <c r="F186" t="s">
@@ -6925,14 +6934,14 @@
       <c r="C187" t="s">
         <v>624</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="3" t="s">
         <v>624</v>
       </c>
       <c r="H187" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6942,7 +6951,7 @@
       <c r="C188" t="s">
         <v>627</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="3" t="s">
         <v>628</v>
       </c>
       <c r="F188" t="s">
@@ -6952,7 +6961,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6962,7 +6971,7 @@
       <c r="C189" t="s">
         <v>631</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="3" t="s">
         <v>632</v>
       </c>
       <c r="H189" t="s">
@@ -6979,14 +6988,14 @@
       <c r="C190" t="s">
         <v>635</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="3" t="s">
         <v>635</v>
       </c>
       <c r="H190" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6996,7 +7005,7 @@
       <c r="C191" t="s">
         <v>637</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="3" t="s">
         <v>638</v>
       </c>
       <c r="H191" t="s">
@@ -7013,14 +7022,14 @@
       <c r="C192" t="s">
         <v>641</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="3" t="s">
         <v>642</v>
       </c>
       <c r="H192" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -7030,7 +7039,7 @@
       <c r="C193" t="s">
         <v>645</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="3" t="s">
         <v>646</v>
       </c>
       <c r="F193" t="s">
@@ -7050,14 +7059,14 @@
       <c r="C194" t="s">
         <v>649</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="3" t="s">
         <v>649</v>
       </c>
       <c r="H194" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -7067,7 +7076,7 @@
       <c r="C195" t="s">
         <v>652</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="3" t="s">
         <v>653</v>
       </c>
       <c r="H195" t="s">
@@ -7084,7 +7093,7 @@
       <c r="C196" t="s">
         <v>656</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="3" t="s">
         <v>657</v>
       </c>
       <c r="F196" t="s">
@@ -7094,7 +7103,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -7104,14 +7113,14 @@
       <c r="C197" t="s">
         <v>659</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="3" t="s">
         <v>660</v>
       </c>
       <c r="H197" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:8" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -7121,7 +7130,7 @@
       <c r="C198" t="s">
         <v>663</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="3" t="s">
         <v>664</v>
       </c>
       <c r="F198" t="s">
@@ -7131,7 +7140,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:8" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -7141,7 +7150,7 @@
       <c r="C199" t="s">
         <v>667</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="3" t="s">
         <v>668</v>
       </c>
       <c r="F199" t="s">
@@ -7161,7 +7170,7 @@
       <c r="C200" t="s">
         <v>671</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="3" t="s">
         <v>672</v>
       </c>
       <c r="H200" t="s">
@@ -7178,14 +7187,14 @@
       <c r="C201" t="s">
         <v>674</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="3" t="s">
         <v>675</v>
       </c>
       <c r="H201" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -7195,7 +7204,7 @@
       <c r="C202" t="s">
         <v>677</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="3" t="s">
         <v>678</v>
       </c>
       <c r="F202" t="s">
@@ -7205,7 +7214,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -7215,7 +7224,7 @@
       <c r="C203" t="s">
         <v>681</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="3" t="s">
         <v>682</v>
       </c>
       <c r="F203" t="s">
@@ -7225,7 +7234,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:8" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -7235,7 +7244,7 @@
       <c r="C204" t="s">
         <v>685</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="3" t="s">
         <v>686</v>
       </c>
       <c r="F204" t="s">
@@ -7255,14 +7264,14 @@
       <c r="C205" t="s">
         <v>689</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="3" t="s">
         <v>689</v>
       </c>
       <c r="H205" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:8" ht="408" x14ac:dyDescent="0.4">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -7272,7 +7281,7 @@
       <c r="C206" t="s">
         <v>691</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="3" t="s">
         <v>692</v>
       </c>
       <c r="F206" t="s">
@@ -7282,7 +7291,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -7292,7 +7301,7 @@
       <c r="C207" t="s">
         <v>695</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="3" t="s">
         <v>696</v>
       </c>
       <c r="F207" t="s">
@@ -7302,7 +7311,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:8" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7312,7 +7321,7 @@
       <c r="C208" t="s">
         <v>698</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="3" t="s">
         <v>699</v>
       </c>
       <c r="F208" t="s">
@@ -7332,7 +7341,7 @@
       <c r="C209" t="s">
         <v>702</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="3" t="s">
         <v>702</v>
       </c>
       <c r="H209" t="s">
@@ -7349,7 +7358,7 @@
       <c r="C210" t="s">
         <v>704</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="3" t="s">
         <v>705</v>
       </c>
       <c r="F210" t="s">
@@ -7369,7 +7378,7 @@
       <c r="C211" t="s">
         <v>707</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="3" t="s">
         <v>707</v>
       </c>
       <c r="H211" t="s">
@@ -7386,14 +7395,14 @@
       <c r="C212" t="s">
         <v>710</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="3" t="s">
         <v>710</v>
       </c>
       <c r="H212" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:8" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7403,7 +7412,7 @@
       <c r="C213" t="s">
         <v>712</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="3" t="s">
         <v>713</v>
       </c>
       <c r="F213" t="s">
@@ -7423,14 +7432,14 @@
       <c r="C214" t="s">
         <v>715</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="3" t="s">
         <v>715</v>
       </c>
       <c r="H214" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:8" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -7440,7 +7449,7 @@
       <c r="C215" t="s">
         <v>717</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="3" t="s">
         <v>718</v>
       </c>
       <c r="H215" t="s">
@@ -7457,7 +7466,7 @@
       <c r="C216" t="s">
         <v>721</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="3" t="s">
         <v>721</v>
       </c>
       <c r="H216" t="s">
@@ -7474,14 +7483,14 @@
       <c r="C217" t="s">
         <v>724</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="3" t="s">
         <v>724</v>
       </c>
       <c r="H217" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:8" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -7491,7 +7500,7 @@
       <c r="C218" t="s">
         <v>726</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="3" t="s">
         <v>727</v>
       </c>
       <c r="F218" t="s">
@@ -7511,7 +7520,7 @@
       <c r="C219" t="s">
         <v>729</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="3" t="s">
         <v>729</v>
       </c>
       <c r="H219" t="s">
@@ -7528,14 +7537,14 @@
       <c r="C220" t="s">
         <v>732</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="3" t="s">
         <v>733</v>
       </c>
       <c r="H220" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:8" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -7545,7 +7554,7 @@
       <c r="C221" t="s">
         <v>736</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="3" t="s">
         <v>737</v>
       </c>
       <c r="F221" t="s">
@@ -7555,7 +7564,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:8" ht="204" x14ac:dyDescent="0.4">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -7565,7 +7574,7 @@
       <c r="C222" t="s">
         <v>739</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="3" t="s">
         <v>740</v>
       </c>
       <c r="F222" t="s">
@@ -7585,14 +7594,14 @@
       <c r="C223" t="s">
         <v>742</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="3" t="s">
         <v>742</v>
       </c>
       <c r="H223" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -7602,7 +7611,7 @@
       <c r="C224" t="s">
         <v>745</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="3" t="s">
         <v>746</v>
       </c>
       <c r="F224" t="s">
@@ -7622,14 +7631,14 @@
       <c r="C225" t="s">
         <v>748</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="3" t="s">
         <v>748</v>
       </c>
       <c r="H225" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -7639,7 +7648,7 @@
       <c r="C226" t="s">
         <v>751</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="3" t="s">
         <v>752</v>
       </c>
       <c r="H226" t="s">
@@ -7656,14 +7665,14 @@
       <c r="C227" t="s">
         <v>755</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="3" t="s">
         <v>755</v>
       </c>
       <c r="H227" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:8" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -7673,14 +7682,14 @@
       <c r="C228" t="s">
         <v>758</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="3" t="s">
         <v>759</v>
       </c>
       <c r="H228" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -7690,7 +7699,7 @@
       <c r="C229" t="s">
         <v>761</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="3" t="s">
         <v>762</v>
       </c>
       <c r="F229" t="s">
@@ -7710,14 +7719,14 @@
       <c r="C230" t="s">
         <v>764</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="3" t="s">
         <v>764</v>
       </c>
       <c r="H230" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:8" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -7727,14 +7736,14 @@
       <c r="C231" t="s">
         <v>767</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="3" t="s">
         <v>768</v>
       </c>
       <c r="H231" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -7744,7 +7753,7 @@
       <c r="C232" t="s">
         <v>771</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="3" t="s">
         <v>772</v>
       </c>
       <c r="H232" t="s">
@@ -7761,14 +7770,14 @@
       <c r="C233" t="s">
         <v>775</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="3" t="s">
         <v>775</v>
       </c>
       <c r="H233" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -7778,7 +7787,7 @@
       <c r="C234" t="s">
         <v>778</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="3" t="s">
         <v>779</v>
       </c>
       <c r="F234" t="s">
@@ -7788,7 +7797,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -7798,7 +7807,7 @@
       <c r="C235" t="s">
         <v>782</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="3" t="s">
         <v>783</v>
       </c>
       <c r="F235" t="s">
@@ -7818,7 +7827,7 @@
       <c r="C236" t="s">
         <v>785</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="3" t="s">
         <v>785</v>
       </c>
       <c r="H236" t="s">
@@ -7835,7 +7844,7 @@
       <c r="C237" t="s">
         <v>787</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="3" t="s">
         <v>788</v>
       </c>
       <c r="H237" t="s">
@@ -7852,14 +7861,14 @@
       <c r="C238" t="s">
         <v>790</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="3" t="s">
         <v>790</v>
       </c>
       <c r="H238" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -7869,7 +7878,7 @@
       <c r="C239" t="s">
         <v>792</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="3" t="s">
         <v>793</v>
       </c>
       <c r="H239" t="s">
@@ -7886,14 +7895,14 @@
       <c r="C240" t="s">
         <v>796</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="3" t="s">
         <v>796</v>
       </c>
       <c r="H240" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -7903,7 +7912,7 @@
       <c r="C241" t="s">
         <v>799</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="3" t="s">
         <v>800</v>
       </c>
       <c r="F241" t="s">
@@ -7913,7 +7922,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -7923,7 +7932,7 @@
       <c r="C242" t="s">
         <v>803</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="3" t="s">
         <v>804</v>
       </c>
       <c r="F242" t="s">
@@ -7943,7 +7952,7 @@
       <c r="C243" t="s">
         <v>807</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="3" t="s">
         <v>807</v>
       </c>
       <c r="H243" t="s">
@@ -7960,14 +7969,14 @@
       <c r="C244" t="s">
         <v>810</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="3" t="s">
         <v>811</v>
       </c>
       <c r="H244" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -7977,14 +7986,14 @@
       <c r="C245" t="s">
         <v>813</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="3" t="s">
         <v>814</v>
       </c>
       <c r="H245" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -7994,7 +8003,7 @@
       <c r="C246" t="s">
         <v>817</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D246" s="3" t="s">
         <v>818</v>
       </c>
       <c r="F246" t="s">
@@ -8004,7 +8013,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -8014,7 +8023,7 @@
       <c r="C247" t="s">
         <v>821</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="3" t="s">
         <v>822</v>
       </c>
       <c r="F247" t="s">
@@ -8034,7 +8043,7 @@
       <c r="C248" t="s">
         <v>824</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="3" t="s">
         <v>824</v>
       </c>
       <c r="H248" t="s">
@@ -8051,7 +8060,7 @@
       <c r="C249" t="s">
         <v>826</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="3" t="s">
         <v>826</v>
       </c>
       <c r="H249" t="s">
@@ -8068,7 +8077,7 @@
       <c r="C250" t="s">
         <v>828</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="3" t="s">
         <v>829</v>
       </c>
       <c r="H250" t="s">
@@ -8085,14 +8094,14 @@
       <c r="C251" t="s">
         <v>832</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D251" s="3" t="s">
         <v>833</v>
       </c>
       <c r="H251" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -8102,7 +8111,7 @@
       <c r="C252" t="s">
         <v>836</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D252" s="3" t="s">
         <v>837</v>
       </c>
       <c r="F252" t="s">
@@ -8112,7 +8121,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -8122,7 +8131,7 @@
       <c r="C253" t="s">
         <v>839</v>
       </c>
-      <c r="D253" t="s">
+      <c r="D253" s="3" t="s">
         <v>840</v>
       </c>
       <c r="F253" t="s">
@@ -8132,7 +8141,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -8142,14 +8151,14 @@
       <c r="C254" t="s">
         <v>842</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D254" s="3" t="s">
         <v>843</v>
       </c>
       <c r="H254" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -8159,7 +8168,7 @@
       <c r="C255" t="s">
         <v>845</v>
       </c>
-      <c r="D255" t="s">
+      <c r="D255" s="3" t="s">
         <v>846</v>
       </c>
       <c r="F255" t="s">
@@ -8179,14 +8188,14 @@
       <c r="C256" t="s">
         <v>849</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D256" s="3" t="s">
         <v>849</v>
       </c>
       <c r="H256" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:8" ht="320.60000000000002" x14ac:dyDescent="0.4">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -8196,7 +8205,7 @@
       <c r="C257" t="s">
         <v>851</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="3" t="s">
         <v>852</v>
       </c>
       <c r="H257" t="s">
@@ -8213,7 +8222,7 @@
       <c r="C258" t="s">
         <v>854</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="3" t="s">
         <v>855</v>
       </c>
       <c r="F258" t="s">
@@ -8233,14 +8242,14 @@
       <c r="C259" t="s">
         <v>857</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" s="3" t="s">
         <v>857</v>
       </c>
       <c r="H259" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -8250,7 +8259,7 @@
       <c r="C260" t="s">
         <v>859</v>
       </c>
-      <c r="D260" t="s">
+      <c r="D260" s="3" t="s">
         <v>860</v>
       </c>
       <c r="F260" t="s">
@@ -8270,14 +8279,14 @@
       <c r="C261" t="s">
         <v>862</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="3" t="s">
         <v>862</v>
       </c>
       <c r="H261" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -8287,7 +8296,7 @@
       <c r="C262" t="s">
         <v>864</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="3" t="s">
         <v>865</v>
       </c>
       <c r="F262" t="s">
@@ -8297,7 +8306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -8307,14 +8316,14 @@
       <c r="C263" t="s">
         <v>867</v>
       </c>
-      <c r="D263" t="s">
+      <c r="D263" s="3" t="s">
         <v>868</v>
       </c>
       <c r="H263" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -8324,7 +8333,7 @@
       <c r="C264" t="s">
         <v>870</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D264" s="3" t="s">
         <v>871</v>
       </c>
       <c r="H264" t="s">
@@ -8341,7 +8350,7 @@
       <c r="C265" t="s">
         <v>874</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D265" s="3" t="s">
         <v>875</v>
       </c>
       <c r="F265" t="s">
@@ -8361,7 +8370,7 @@
       <c r="C266" t="s">
         <v>877</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="3" t="s">
         <v>877</v>
       </c>
       <c r="H266" t="s">
@@ -8378,14 +8387,14 @@
       <c r="C267" t="s">
         <v>880</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D267" s="3" t="s">
         <v>881</v>
       </c>
       <c r="H267" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -8395,7 +8404,7 @@
       <c r="C268" t="s">
         <v>883</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D268" s="3" t="s">
         <v>884</v>
       </c>
       <c r="F268" t="s">
@@ -8405,7 +8414,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:8" ht="204" x14ac:dyDescent="0.4">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -8415,7 +8424,7 @@
       <c r="C269" t="s">
         <v>886</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="3" t="s">
         <v>887</v>
       </c>
       <c r="H269" t="s">
@@ -8432,7 +8441,7 @@
       <c r="C270" t="s">
         <v>889</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D270" s="3" t="s">
         <v>890</v>
       </c>
       <c r="H270" t="s">
@@ -8449,7 +8458,7 @@
       <c r="C271" t="s">
         <v>892</v>
       </c>
-      <c r="D271" t="s">
+      <c r="D271" s="3" t="s">
         <v>892</v>
       </c>
       <c r="H271" t="s">
@@ -8466,7 +8475,7 @@
       <c r="C272" t="s">
         <v>894</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="3" t="s">
         <v>894</v>
       </c>
       <c r="H272" t="s">
@@ -8483,7 +8492,7 @@
       <c r="C273" t="s">
         <v>896</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="3" t="s">
         <v>897</v>
       </c>
       <c r="H273" t="s">
@@ -8500,7 +8509,7 @@
       <c r="C274" t="s">
         <v>899</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D274" s="3" t="s">
         <v>900</v>
       </c>
       <c r="F274" t="s">
@@ -8510,7 +8519,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -8520,7 +8529,7 @@
       <c r="C275" t="s">
         <v>902</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="3" t="s">
         <v>903</v>
       </c>
       <c r="F275" t="s">
@@ -8540,14 +8549,14 @@
       <c r="C276" t="s">
         <v>905</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="3" t="s">
         <v>905</v>
       </c>
       <c r="H276" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:8" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -8557,7 +8566,7 @@
       <c r="C277" t="s">
         <v>907</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="3" t="s">
         <v>908</v>
       </c>
       <c r="H277" t="s">
@@ -8574,7 +8583,7 @@
       <c r="C278" t="s">
         <v>910</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="3" t="s">
         <v>910</v>
       </c>
       <c r="H278" t="s">
@@ -8591,14 +8600,14 @@
       <c r="C279" t="s">
         <v>912</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="3" t="s">
         <v>913</v>
       </c>
       <c r="H279" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -8608,7 +8617,7 @@
       <c r="C280" t="s">
         <v>915</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="3" t="s">
         <v>916</v>
       </c>
       <c r="H280" t="s">
@@ -8625,14 +8634,14 @@
       <c r="C281" t="s">
         <v>919</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="3" t="s">
         <v>919</v>
       </c>
       <c r="H281" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -8642,14 +8651,14 @@
       <c r="C282" t="s">
         <v>922</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="3" t="s">
         <v>923</v>
       </c>
       <c r="H282" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:8" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -8659,7 +8668,7 @@
       <c r="C283" t="s">
         <v>925</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="3" t="s">
         <v>926</v>
       </c>
       <c r="F283" t="s">
@@ -8679,14 +8688,14 @@
       <c r="C284" t="s">
         <v>928</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="3" t="s">
         <v>928</v>
       </c>
       <c r="H284" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -8696,7 +8705,7 @@
       <c r="C285" t="s">
         <v>931</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="3" t="s">
         <v>932</v>
       </c>
       <c r="F285" t="s">
@@ -8716,7 +8725,7 @@
       <c r="C286" t="s">
         <v>934</v>
       </c>
-      <c r="D286" t="s">
+      <c r="D286" s="3" t="s">
         <v>935</v>
       </c>
       <c r="F286" t="s">
@@ -8736,14 +8745,14 @@
       <c r="C287" t="s">
         <v>937</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="3" t="s">
         <v>937</v>
       </c>
       <c r="H287" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -8753,7 +8762,7 @@
       <c r="C288" t="s">
         <v>939</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D288" s="3" t="s">
         <v>940</v>
       </c>
       <c r="F288" t="s">
@@ -8773,7 +8782,7 @@
       <c r="C289" t="s">
         <v>942</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D289" s="3" t="s">
         <v>943</v>
       </c>
       <c r="H289" t="s">
@@ -8790,14 +8799,14 @@
       <c r="C290" t="s">
         <v>945</v>
       </c>
-      <c r="D290" t="s">
+      <c r="D290" s="3" t="s">
         <v>945</v>
       </c>
       <c r="H290" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:8" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -8807,7 +8816,7 @@
       <c r="C291" t="s">
         <v>948</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="3" t="s">
         <v>949</v>
       </c>
       <c r="F291" t="s">
@@ -8827,7 +8836,7 @@
       <c r="C292" t="s">
         <v>951</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D292" s="3" t="s">
         <v>952</v>
       </c>
       <c r="H292" t="s">
@@ -8844,14 +8853,14 @@
       <c r="C293" t="s">
         <v>954</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D293" s="3" t="s">
         <v>954</v>
       </c>
       <c r="H293" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:8" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -8861,7 +8870,7 @@
       <c r="C294" t="s">
         <v>956</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D294" s="3" t="s">
         <v>957</v>
       </c>
       <c r="H294" t="s">
@@ -8878,7 +8887,7 @@
       <c r="C295" t="s">
         <v>960</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D295" s="3" t="s">
         <v>960</v>
       </c>
       <c r="H295" t="s">
@@ -8895,14 +8904,14 @@
       <c r="C296" t="s">
         <v>962</v>
       </c>
-      <c r="D296" t="s">
+      <c r="D296" s="3" t="s">
         <v>963</v>
       </c>
       <c r="H296" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:8" ht="408" x14ac:dyDescent="0.4">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -8912,7 +8921,7 @@
       <c r="C297" t="s">
         <v>965</v>
       </c>
-      <c r="D297" t="s">
+      <c r="D297" s="3" t="s">
         <v>966</v>
       </c>
       <c r="F297" t="s">
@@ -8922,7 +8931,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -8932,14 +8941,14 @@
       <c r="C298" t="s">
         <v>969</v>
       </c>
-      <c r="D298" t="s">
+      <c r="D298" s="3" t="s">
         <v>970</v>
       </c>
       <c r="H298" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:8" ht="102" x14ac:dyDescent="0.4">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -8949,7 +8958,7 @@
       <c r="C299" t="s">
         <v>973</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" s="3" t="s">
         <v>974</v>
       </c>
       <c r="H299" t="s">
@@ -8966,7 +8975,7 @@
       <c r="C300" t="s">
         <v>977</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D300" s="3" t="s">
         <v>978</v>
       </c>
       <c r="H300" t="s">
@@ -8983,7 +8992,7 @@
       <c r="C301" t="s">
         <v>981</v>
       </c>
-      <c r="D301" t="s">
+      <c r="D301" s="3" t="s">
         <v>981</v>
       </c>
       <c r="H301" t="s">
@@ -9000,7 +9009,7 @@
       <c r="C302" t="s">
         <v>983</v>
       </c>
-      <c r="D302" t="s">
+      <c r="D302" s="3" t="s">
         <v>983</v>
       </c>
       <c r="H302" t="s">
@@ -9017,14 +9026,14 @@
       <c r="C303" t="s">
         <v>986</v>
       </c>
-      <c r="D303" t="s">
+      <c r="D303" s="3" t="s">
         <v>986</v>
       </c>
       <c r="H303" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -9034,14 +9043,14 @@
       <c r="C304" t="s">
         <v>989</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D304" s="3" t="s">
         <v>990</v>
       </c>
       <c r="H304" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:8" ht="204" x14ac:dyDescent="0.4">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -9051,7 +9060,7 @@
       <c r="C305" t="s">
         <v>992</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D305" s="3" t="s">
         <v>993</v>
       </c>
       <c r="F305" t="s">
@@ -9061,7 +9070,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:8" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -9071,7 +9080,7 @@
       <c r="C306" t="s">
         <v>995</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D306" s="3" t="s">
         <v>996</v>
       </c>
       <c r="H306" t="s">
@@ -9088,14 +9097,14 @@
       <c r="C307" t="s">
         <v>998</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D307" s="3" t="s">
         <v>998</v>
       </c>
       <c r="H307" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:8" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -9105,14 +9114,14 @@
       <c r="C308" t="s">
         <v>1000</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D308" s="3" t="s">
         <v>1001</v>
       </c>
       <c r="H308" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -9122,7 +9131,7 @@
       <c r="C309" t="s">
         <v>1003</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" s="3" t="s">
         <v>1004</v>
       </c>
       <c r="F309" t="s">
@@ -9132,7 +9141,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -9142,7 +9151,7 @@
       <c r="C310" t="s">
         <v>1007</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D310" s="3" t="s">
         <v>1008</v>
       </c>
       <c r="F310" t="s">
@@ -9152,7 +9161,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -9162,7 +9171,7 @@
       <c r="C311" t="s">
         <v>1011</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D311" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="F311" t="s">
@@ -9182,7 +9191,7 @@
       <c r="C312" t="s">
         <v>1014</v>
       </c>
-      <c r="D312" t="s">
+      <c r="D312" s="3" t="s">
         <v>1015</v>
       </c>
       <c r="F312" t="s">
@@ -9192,7 +9201,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -9202,14 +9211,14 @@
       <c r="C313" t="s">
         <v>1018</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D313" s="3" t="s">
         <v>1019</v>
       </c>
       <c r="H313" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:8" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -9219,7 +9228,7 @@
       <c r="C314" t="s">
         <v>1021</v>
       </c>
-      <c r="D314" t="s">
+      <c r="D314" s="3" t="s">
         <v>1022</v>
       </c>
       <c r="F314" t="s">
@@ -9229,7 +9238,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -9239,7 +9248,7 @@
       <c r="C315" t="s">
         <v>1025</v>
       </c>
-      <c r="D315" t="s">
+      <c r="D315" s="3" t="s">
         <v>1026</v>
       </c>
     </row>

</xml_diff>